<commit_message>
Updated reviewer response table.
</commit_message>
<xml_diff>
--- a/Submissions/2 Reviewer Comments and Response/Lighting Paper Review Response 2.xlsx
+++ b/Submissions/2 Reviewer Comments and Response/Lighting Paper Review Response 2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earpebr\Github\LightingPaper2020\Submissions\2 Reviewer Comments and Response\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/2 Reviewer Comments and Response/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3E3D8B-8A36-0C43-A74E-26E6AE349E53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="48680" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,72 +23,119 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Paul Brockway</author>
   </authors>
   <commentList>
-    <comment ref="E11" authorId="0" shapeId="0">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Paul Brockway:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-moving a Table around doesn’t seem to tally with their comment. They just want the symbols from table 8 to be in the nomenclature?</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>moving a Table around doesn’t seem to tally with their comment. They just want the symbols from table 8 to be in the nomenclature?</t>
         </r>
       </text>
     </comment>
-    <comment ref="E29" authorId="0" shapeId="0">
+    <comment ref="E29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Paul Brockway:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-is thre reivewer mis-writing? Are they meaning that the 2nd law only holds for isolated systems? And therefore it doesn’t appy if we have a closed systems (only energy is exchnaged). 
-Wiki talks of the 2nd law and the isolated system (matter and energy can be exchnaged)https://en.wikipedia.org/wiki/Second_law_of_thermodynamics
-but i am sure hte 2nd law is universal, and even if we just had an siolated systems (energy exchnage only) then the 2nd law woudl hold
-simnple wiki talks of a closed system https://simple.wikipedia.org/wiki/Second_law_of_thermodynamics
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">is thre reivewer mis-writing? Are they meaning that the 2nd law only holds for isolated systems? And therefore it doesn’t appy if we have a closed systems (only energy is exchnaged). 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Wiki talks of the 2nd law and the isolated system (matter and energy can be exchnaged)https://en.wikipedia.org/wiki/Second_law_of_thermodynamics
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but i am sure hte 2nd law is universal, and even if we just had an siolated systems (energy exchnage only) then the 2nd law woudl hold
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">simnple wiki talks of a closed system https://simple.wikipedia.org/wiki/Second_law_of_thermodynamics
 </t>
         </r>
       </text>
@@ -97,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>The Energy and Exergy of Light</t>
   </si>
@@ -189,9 +237,6 @@
     <t>3.10</t>
   </si>
   <si>
-    <t>HELP!</t>
-  </si>
-  <si>
     <t>ZM</t>
   </si>
   <si>
@@ -242,11 +287,14 @@
   <si>
     <t>ZM: I believe reviewer three's comment to be wrong here. Paoli &amp; Cullen use four stages of energy loss to produce the figure 284-350 lm/W (Spectral Efficiency, Driver Efficiency, Wall Plug Efficiency, and Optical Efficiency - see right). The Luminous Efficacy of radiation that he refers to is the bottom row of table 5 (see right) - the spectral efficacy. The luminous effiacy of a source which he refers to is the 284-250 lm/W which includes all of the aformentioned stages.</t>
   </si>
+  <si>
+    <t>Perhaps we should back away from 2nd Law language and consider exergy accounting language. We are actually doing exergy accounting, anyway.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -279,17 +327,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -391,7 +439,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3192,7 +3239,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3267,7 +3313,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6715,45 +6760,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="2"/>
-    <col min="2" max="2" width="71.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="57.75" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="2"/>
-    <col min="5" max="5" width="48.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="44.75" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.75" style="2"/>
+    <col min="1" max="1" width="10.6640625" style="2"/>
+    <col min="2" max="2" width="71.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="2"/>
+    <col min="5" max="5" width="48.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
@@ -6767,10 +6812,10 @@
         <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -6781,10 +6826,10 @@
         <v>21</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>1.2</v>
       </c>
@@ -6795,15 +6840,15 @@
         <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
@@ -6817,10 +6862,10 @@
         <v>22</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2.1</v>
       </c>
@@ -6834,7 +6879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -6848,12 +6893,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
@@ -6867,10 +6912,10 @@
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>3.1</v>
       </c>
@@ -6884,7 +6929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>3.2</v>
       </c>
@@ -6898,7 +6943,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>3.3</v>
       </c>
@@ -6912,18 +6957,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>3.4</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="D29" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="E29" s="3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>3.5</v>
       </c>
@@ -6931,16 +6979,16 @@
         <v>14</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="178.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="178.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>3.6</v>
       </c>
@@ -6948,16 +6996,16 @@
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>3.7</v>
       </c>
@@ -6965,30 +7013,30 @@
         <v>16</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="161.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="161.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>3.8</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>3.9</v>
       </c>
@@ -6999,10 +7047,10 @@
         <v>21</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="241.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="241.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>29</v>
       </c>
@@ -7010,16 +7058,16 @@
         <v>18</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>3.11</v>
       </c>
@@ -7027,13 +7075,13 @@
         <v>19</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nomenclature all in one table.
</commit_message>
<xml_diff>
--- a/Submissions/2 Reviewer Comments and Response/Lighting Paper Review Response 2.xlsx
+++ b/Submissions/2 Reviewer Comments and Response/Lighting Paper Review Response 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/2 Reviewer Comments and Response/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7154E4-77D4-3E4A-A5A9-4BBAE642BD44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0175C5D1-C109-EF49-8684-9DB753262200}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28880" yWindow="460" windowWidth="25680" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>The Energy and Exergy of Light</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>Split equations to their own lines.</t>
+  </si>
+  <si>
+    <t>Comma inserted, as suggested. Thanks!</t>
+  </si>
+  <si>
+    <t>The section in question seems right to us. The sentence says, "Thus, light is EM radiation … sensitivity." The parenthetical sentence is complete as writtten. "(See Figure 1.)" is an imperative sentence with implied subject "You". No changes were made in response to this particular suggestion. However, at the reviewer's suggestion, we did another thorough proofread immediately prior to submission.</t>
+  </si>
+  <si>
+    <t>DONE.</t>
   </si>
 </sst>
 </file>
@@ -5082,8 +5091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AMK36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="A18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5185,31 +5194,43 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="A18" s="8">
         <v>2.1</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="C18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="F18" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+    <row r="19" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="C19" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="8" t="s">
         <v>16</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
More responses to reviewers.
</commit_message>
<xml_diff>
--- a/Submissions/2 Reviewer Comments and Response/Lighting Paper Review Response 2.xlsx
+++ b/Submissions/2 Reviewer Comments and Response/Lighting Paper Review Response 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/2 Reviewer Comments and Response/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0175C5D1-C109-EF49-8684-9DB753262200}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8204DD-1237-2D47-9D83-52EFA133B671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28880" yWindow="460" windowWidth="25680" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>The Energy and Exergy of Light</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>DONE.</t>
+  </si>
+  <si>
+    <t>We combined all nomenclature into a single table.</t>
+  </si>
+  <si>
+    <t>Table 8 is placed automatically by LaTeX. The proofs will almost certainly look different, so there is no need to address placement issues at this time.</t>
   </si>
 </sst>
 </file>
@@ -417,9 +423,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -431,6 +434,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5091,8 +5097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AMK36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="A18:F18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5144,31 +5150,43 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="F11" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
         <v>1.2</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="8" t="s">
         <v>13</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
@@ -5194,42 +5212,42 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="8">
+      <c r="A18" s="7">
         <v>2.1</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="119" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5259,13 +5277,13 @@
       <c r="A26" s="1">
         <v>3.1</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5273,13 +5291,13 @@
       <c r="A27" s="1">
         <v>3.2</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5287,13 +5305,13 @@
       <c r="A28" s="1">
         <v>3.3</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5301,13 +5319,13 @@
       <c r="A29" s="1">
         <v>3.4</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5315,13 +5333,13 @@
       <c r="A30" s="1">
         <v>3.5</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -5332,16 +5350,16 @@
       <c r="A31" s="1">
         <v>3.6</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5349,73 +5367,73 @@
       <c r="A32" s="1">
         <v>3.7</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="272" x14ac:dyDescent="0.2">
-      <c r="A33" s="8">
+      <c r="A33" s="7">
         <v>3.8</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8">
+      <c r="A34" s="7">
         <v>3.9</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="241.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5423,16 +5441,16 @@
       <c r="A36" s="1">
         <v>3.11</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated review response spreadsheet.
</commit_message>
<xml_diff>
--- a/Submissions/2 Reviewer Comments and Response/Lighting Paper Review Response 2.xlsx
+++ b/Submissions/2 Reviewer Comments and Response/Lighting Paper Review Response 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Submissions\2 Reviewer Comments and Response\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99A2B6C-BA7B-43AA-9517-A79717104EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7265E326-8488-4CD4-92DD-BF8387580294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4596" yWindow="2820" windowWidth="9216" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
   <si>
     <t>The Energy and Exergy of Light</t>
   </si>
@@ -260,9 +260,6 @@
     <t xml:space="preserve">The paragraph in lines 86-91 is described in a very confusing expression. The luminous efficacy 284-350 lm/W is not including any energy loss, and just focuses on the effect of the photopic luminous weighting function itself only. For the completeness, it is called as THE LUMINOUS EFFICACY OF RADIATION. On the other hand, the electric wall-plugging efficiency, the internal efficiency, the extraction efficiency, the optic utilization factor are combined into THE LUMINOUS EFFICACY OF A SOURCE for the energy conversion efficiency. </t>
   </si>
   <si>
-    <t>Diagnose the problem by discerning where the confusion emerges from this paragraph. Rewrite for clarity.</t>
-  </si>
-  <si>
     <t xml:space="preserve">In the section of 2.1.1, all the upper dots over the variables should be deleted. It discusses on the energy conversion, rather than on the temporal change rate of the energies. </t>
   </si>
   <si>
@@ -282,9 +279,6 @@
   </si>
   <si>
     <t xml:space="preserve">Will the overall average values (0.956 and 1.36) used in Eq. (44) work for all lamps? and Why? </t>
-  </si>
-  <si>
-    <t>Add a sentence or two that narrows the claim to the lamps we studied. We could say that "in the absence of any better information, these values are recommended.</t>
   </si>
   <si>
     <t xml:space="preserve">There are two typical meanings for overdots in the engineering literature. (a) The overdot can signify a first derivative with respect to time, as is typical in noise and vibration literature. An example would be x_dot meaning the first derivative of position (x) with respect to time, or velocity.  (b) The overdot can also signify a steady state rate, as is typical in the energy literature. An example of this second meaning is Q_dot for a heat transfer rate (J/s or watts). We are using the overdot in the second sense to signify rates of energy and exergy flows during steady-state operation. 
@@ -331,6 +325,12 @@
   </si>
   <si>
     <t>I have emphasised that Paoli &amp; Cullen's estimate of 284-350 lm/W includes all of the reviewers aforemented stages, which Paoli &amp; Cullen term: Driver efficiency, Wall Plug efficiency, Optical efficiency, and Spectral efficiency. The estimate of 284-350 lm/W is therefore the luminous efficacy of the source. The luminous efficacy of radiation, which refers to the effect of the photopic luminosity function alone is termed the Spectral efficiency by Paoli &amp; Cullen, and equal to 348-414 lm/W. This information can be found in Section 2.2.2 of the SI of Paoli &amp; Cullen (2020).</t>
+  </si>
+  <si>
+    <t>We have added the coreect CIE reference for the 10 deg CMF function.</t>
+  </si>
+  <si>
+    <t>Add a sentence or two that narrows the claim to the lamps we studied. We could say that "in the absence of any better information, these values are recommended. ZM: I have not added any further text as I believe we have covered this ground sufficiently.</t>
   </si>
 </sst>
 </file>
@@ -924,6 +924,168 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1249680</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B40757-0F56-4B2A-BE0C-6CFD3BA359E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12702540" cy="13997940"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1249680</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEE47FA2-C683-4BF5-8174-F84FDD16CAAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12702540" cy="13997940"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1249680</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73C85948-531A-4338-997B-D55FD67D63DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12702540" cy="13997940"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1226,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AMK36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1286,7 +1448,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>10</v>
@@ -1295,7 +1457,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1306,7 +1468,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>10</v>
@@ -1315,7 +1477,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
@@ -1348,7 +1510,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>10</v>
@@ -1357,7 +1519,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
@@ -1368,7 +1530,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>10</v>
@@ -1377,7 +1539,7 @@
         <v>16</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
@@ -1466,7 +1628,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>28</v>
@@ -1475,7 +1637,7 @@
         <v>29</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="178.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1486,16 +1648,16 @@
         <v>30</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.3">
@@ -1506,16 +1668,16 @@
         <v>31</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="265.2" x14ac:dyDescent="0.3">
@@ -1523,19 +1685,19 @@
         <v>3.8</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1543,39 +1705,39 @@
         <v>3.9</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="241.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="C35" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
@@ -1583,19 +1745,19 @@
         <v>3.11</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>